<commit_message>
Add author and homework information to fipponachy.m
</commit_message>
<xml_diff>
--- a/Experiments/Fundamental_physics/RLC_table/data/data.xlsx
+++ b/Experiments/Fundamental_physics/RLC_table/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>f</t>
   </si>
@@ -35,12 +35,15 @@
     <t>元件</t>
   </si>
   <si>
+    <t>特征值</t>
+  </si>
+  <si>
+    <t>单位</t>
+  </si>
+  <si>
     <t>电阻值</t>
   </si>
   <si>
-    <t>units</t>
-  </si>
-  <si>
     <t>谐振频率</t>
   </si>
   <si>
@@ -50,19 +53,25 @@
     <t>Q</t>
   </si>
   <si>
-    <t>10mH电感</t>
-  </si>
-  <si>
-    <t>ohm</t>
+    <t>电感</t>
+  </si>
+  <si>
+    <t>mH</t>
+  </si>
+  <si>
+    <t>Ohm</t>
   </si>
   <si>
     <t>1558hz</t>
   </si>
   <si>
-    <t>1kohm电阻</t>
-  </si>
-  <si>
-    <t>1 uf电容</t>
+    <t>电阻</t>
+  </si>
+  <si>
+    <t>电容</t>
+  </si>
+  <si>
+    <t>uf</t>
   </si>
   <si>
     <t>N/A</t>
@@ -73,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +93,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -115,33 +130,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -455,94 +482,122 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="C2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5">
         <v>14.25</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5">
         <v>0.96</v>
       </c>
-      <c r="F2" s="4">
+      <c r="H2" s="5">
         <v>9.31</v>
       </c>
-      <c r="G2" s="4">
-        <f>E2/F2</f>
+      <c r="I2" s="5">
+        <f>G2/H2</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3">
+      <c r="D3" s="4">
         <v>990</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="9"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -556,15 +611,15 @@
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -577,7 +632,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -585,563 +640,563 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>28</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>1.71</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>9.97</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <f>B2/C2</f>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>-80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>43</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>2.57</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>9.96</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <f>B3/C3</f>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>-75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>58</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>3.35</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>9.93</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <f>B4/C4</f>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>-70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>74</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>4.12</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>9.9</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <f>B5/C5</f>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>-65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>92</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>4.88</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>9.86</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <f>B6/C6</f>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>-60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>111</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>5.56</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>9.82</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <f>B7/C7</f>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>-55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>133</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>6.21</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>9.79</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <f>B8/C8</f>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>-50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>158</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>6.8</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>9.75</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <f>B9/C9</f>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>-45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>187</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>7.33</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>9.72</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <f>B10/C10</f>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>-40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>224</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>7.82</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>9.67</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <f>B11/C11</f>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>-35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>268</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>8.22</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>9.64</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <f>B12/C12</f>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>-30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>328</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="5">
         <v>8.58</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>9.61</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="5">
         <f>B13/C13</f>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>-25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>411</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>8.88</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>9.59</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <f>B14/C14</f>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>-20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>523</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>9.09</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>9.56</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <f>B15/C15</f>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>-15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>734</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>9.24</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>9.5</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <f>B16/C16</f>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>-10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>1028</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="5">
         <v>9.19</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>9.36</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5">
         <f>B17/C17</f>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>-5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>1558</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>9.17</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>9.3</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <f>B18/C18</f>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="4">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>2390</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="5">
         <v>9.13</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <v>9.32</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="5">
         <f>B19/C19</f>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="4">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <v>3370</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="5">
         <v>9.04</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <v>9.33</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="5">
         <f>B20/C20</f>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="4">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>4690</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="5">
         <v>8.86</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <v>9.35</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="5">
         <f>B21/C21</f>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="4">
         <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>6120</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="5">
         <v>8.63</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="5">
         <v>9.37</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="5">
         <f>B22/C22</f>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="4">
         <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="3">
+      <c r="A23" s="4">
         <v>7720</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="5">
         <v>8.32</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="5">
         <v>9.4</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="5">
         <f>B23/C23</f>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="4">
         <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="3">
+      <c r="A24" s="4">
         <v>9400</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="5">
         <v>7.8</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="5">
         <v>9.43</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="5">
         <f>B24/C24</f>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="4">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="3">
+      <c r="A25" s="4">
         <v>11290</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="5">
         <v>7.58</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="5">
         <v>9.46</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="5">
         <f>B25/C25</f>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="4">
         <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="3">
+      <c r="A26" s="4">
         <v>13490</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="5">
         <v>7.12</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="5">
         <v>9.5</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="5">
         <f>B26/C26</f>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="4">
         <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="3">
+      <c r="A27" s="4">
         <v>16137</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="5">
         <v>6.58</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="5">
         <v>9.54</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="5">
         <f>B27/C27</f>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="4">
         <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="3">
+      <c r="A28" s="4">
         <v>19040</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="5">
         <v>6.04</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="5">
         <v>9.58</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="5">
         <f>B28/C28</f>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="4">
         <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="3">
+      <c r="A29" s="4">
         <v>22880</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="5">
         <v>5.41</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="5">
         <v>9.62</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="5">
         <f>B29/C29</f>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="4">
         <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="3">
+      <c r="A30" s="4">
         <v>27480</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="5">
         <v>4.77</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="5">
         <v>9.66</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="5">
         <f>B30/C30</f>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="4">
         <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="3">
+      <c r="A31" s="4">
         <v>33480</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="5">
         <v>4.14</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="5">
         <v>9.69</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="5">
         <f>B31/C31</f>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="4">
         <v>65</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="3">
+      <c r="A32" s="4">
         <v>41980</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="5">
         <v>3.41</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="5">
         <v>9.72</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="5">
         <f>B32/C32</f>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="4">
         <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="3">
+      <c r="A33" s="4">
         <v>53980</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="5">
         <v>2.74</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="5">
         <v>9.77</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="5">
         <f>B33/C33</f>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="4">
         <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="3">
+      <c r="A34" s="4">
         <v>74080</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="5">
         <v>2.04</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="5">
         <v>9.79</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="5">
         <f>B34/C34</f>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="4">
         <v>80</v>
       </c>
     </row>

</xml_diff>